<commit_message>
added data for Justicia 2024 and 2025
</commit_message>
<xml_diff>
--- a/data/Departamento_de_Justicia/djDelitos2023.xlsx
+++ b/data/Departamento_de_Justicia/djDelitos2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Departamento_de_Justicia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A6862C-889A-4BC7-AFCC-ABAC7F47CBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A464DA-42E4-45E7-80DE-5F0EB78002C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,12 +119,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -156,8 +158,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,7 +378,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -416,16 +418,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D2" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" s="2">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F2" s="2">
         <v>9</v>
@@ -435,7 +437,7 @@
       </c>
       <c r="H2">
         <f>SUM(B2:G2)</f>
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -443,16 +445,16 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D3" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2">
         <v>3</v>
@@ -461,8 +463,8 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H15" si="0">SUM(B3:G3)</f>
-        <v>298</v>
+        <f t="shared" ref="H3:H14" si="0">SUM(B3:G3)</f>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -470,13 +472,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D4" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2">
         <v>97</v>
@@ -485,11 +487,11 @@
         <v>8</v>
       </c>
       <c r="G4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -497,26 +499,26 @@
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D5" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E5" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F5" s="2">
         <v>10</v>
       </c>
       <c r="G5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>705</v>
+        <v>699</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -524,26 +526,26 @@
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D6" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -551,26 +553,26 @@
         <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
-        <v>187</v>
+        <v>119</v>
       </c>
       <c r="D7" s="2">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>388</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -578,26 +580,26 @@
         <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="D8" s="2">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="F8" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -605,26 +607,26 @@
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="D9" s="2">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F9" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>291</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -632,26 +634,26 @@
         <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D10" s="2">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2">
         <v>7</v>
       </c>
       <c r="G10" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>422</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -659,10 +661,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="2">
         <v>40</v>
@@ -678,7 +680,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -686,16 +688,16 @@
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D12" s="2">
         <v>79</v>
       </c>
       <c r="E12" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F12" s="2">
         <v>3</v>
@@ -705,7 +707,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -716,23 +718,23 @@
         <v>66</v>
       </c>
       <c r="C13" s="2">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D13" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13" s="2">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F13" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" s="2">
         <v>7</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>798</v>
+        <v>784</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -740,13 +742,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2">
         <v>29</v>
@@ -759,7 +761,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -768,31 +770,31 @@
       </c>
       <c r="B15">
         <f>SUM(B2:B14)</f>
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C15">
         <f t="shared" ref="C15:G15" si="1">SUM(C2:C14)</f>
-        <v>2364</v>
+        <v>2336</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>902</v>
+        <v>888</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>1271</v>
+        <v>1252</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H15">
         <f>SUM(H2:H14)</f>
-        <v>5123</v>
+        <v>5052</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>